<commit_message>
Added multiple Utbildningstillfälle and Utbildningsinstans to both schemas and maps
</commit_message>
<xml_diff>
--- a/INT0001.Ladok2.Events/Src/Files/INT0001.Ladok2.maps.xlsx
+++ b/INT0001.Ladok2.Events/Src/Files/INT0001.Ladok2.maps.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AterbudEvent" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="93">
   <si>
     <t>pnr</t>
   </si>
@@ -284,6 +284,33 @@
   </si>
   <si>
     <t>Hämtas via MySQL anrop (GetSemesters), värdena konverteras till datum</t>
+  </si>
+  <si>
+    <t>../Utbildningstillfalle[1]</t>
+  </si>
+  <si>
+    <t>../Utbildningsinstans[1]</t>
+  </si>
+  <si>
+    <t>../Utbildningstillfalle[2]</t>
+  </si>
+  <si>
+    <t>Första Utbildningstillfället</t>
+  </si>
+  <si>
+    <t>Andra Utbildningstillfället skapas i det fallet ett program finns angivet</t>
+  </si>
+  <si>
+    <t>Fast värde "XXXX"</t>
+  </si>
+  <si>
+    <t>../Utbildningsinstans[2]</t>
+  </si>
+  <si>
+    <t>Andra Utbildningsinstansen skapas i det fallet ett program finns angivet</t>
+  </si>
+  <si>
+    <t>program</t>
   </si>
 </sst>
 </file>
@@ -352,7 +379,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
@@ -360,6 +387,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -370,14 +406,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -677,17 +710,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" t="s">
         <v>44</v>
       </c>
@@ -713,24 +746,24 @@
       <c r="D4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
@@ -739,15 +772,15 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -756,8 +789,8 @@
       <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
@@ -846,17 +879,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" t="s">
         <v>44</v>
       </c>
@@ -879,10 +912,10 @@
       <c r="D4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -891,15 +924,15 @@
       <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
@@ -908,15 +941,15 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -925,8 +958,8 @@
       <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
@@ -935,15 +968,15 @@
       <c r="D10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -955,8 +988,8 @@
       <c r="D12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -965,8 +998,8 @@
       <c r="D13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D14" s="1" t="s">
@@ -1023,17 +1056,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" t="s">
         <v>44</v>
       </c>
@@ -1056,10 +1089,10 @@
       <c r="D4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -1068,15 +1101,15 @@
       <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
@@ -1085,8 +1118,8 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
@@ -1095,15 +1128,15 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1112,8 +1145,8 @@
       <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
@@ -1122,15 +1155,15 @@
       <c r="D11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1142,8 +1175,8 @@
       <c r="D13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1206,17 +1239,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" t="s">
         <v>44</v>
       </c>
@@ -1240,10 +1273,10 @@
       <c r="D4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -1252,15 +1285,15 @@
       <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
@@ -1269,15 +1302,15 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1286,15 +1319,15 @@
       <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1306,8 +1339,8 @@
       <c r="D11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -1316,15 +1349,15 @@
       <c r="D12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1377,7 +1410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1391,17 +1424,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" t="s">
         <v>44</v>
       </c>
@@ -1425,10 +1458,10 @@
       <c r="D4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -1437,15 +1470,15 @@
       <c r="D5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
@@ -1454,15 +1487,15 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1471,8 +1504,8 @@
       <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
@@ -1481,8 +1514,8 @@
       <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1491,31 +1524,31 @@
       <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
@@ -1607,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:F13"/>
+      <selection activeCell="A12" sqref="A12:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1622,17 +1655,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" t="s">
         <v>44</v>
       </c>
@@ -1656,10 +1689,10 @@
       <c r="D4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -1668,15 +1701,15 @@
       <c r="D5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
@@ -1685,8 +1718,8 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
@@ -1695,15 +1728,15 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1712,8 +1745,8 @@
       <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1725,15 +1758,18 @@
       <c r="D11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>87</v>
+      </c>
       <c r="D12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+        <v>84</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1745,8 +1781,8 @@
       <c r="D13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1756,45 +1792,88 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D15" s="1" t="s">
-        <v>49</v>
+    <row r="15" spans="1:6" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="C15" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D18" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D17" s="1" t="s">
+    <row r="20" spans="1:4" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="C20" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D22" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C18" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
         <v>63</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C19" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
         <v>63</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D24" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>0</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D25" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1810,10 +1889,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1822,20 +1901,21 @@
     <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" t="s">
         <v>44</v>
       </c>
@@ -1859,10 +1939,10 @@
       <c r="D4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -1871,15 +1951,15 @@
       <c r="D5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
@@ -1888,8 +1968,8 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
@@ -1898,15 +1978,15 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1915,8 +1995,8 @@
       <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1928,15 +2008,16 @@
       <c r="D11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>87</v>
+      </c>
       <c r="D12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+        <v>84</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1948,8 +2029,6 @@
       <c r="D13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1959,45 +2038,92 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D15" s="1" t="s">
-        <v>49</v>
-      </c>
+    <row r="15" spans="1:6" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="C15" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D18" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D17" s="1" t="s">
+    <row r="20" spans="1:6" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="C20" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20"/>
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D22" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C18" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
         <v>82</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C19" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
         <v>82</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D24" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>0</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D25" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2005,7 +2131,7 @@
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="E4:F13"/>
+    <mergeCell ref="E4:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2028,17 +2154,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" t="s">
         <v>43</v>
       </c>
@@ -2062,10 +2188,10 @@
       <c r="D4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
@@ -2076,8 +2202,8 @@
       <c r="D5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
@@ -2085,8 +2211,8 @@
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
@@ -2097,8 +2223,8 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
@@ -2106,8 +2232,8 @@
       <c r="D8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
@@ -2118,8 +2244,8 @@
       <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
@@ -2128,15 +2254,15 @@
       <c r="D10" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -2145,12 +2271,12 @@
       <c r="D12" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Added Organisation schema to Registrering and Omregistrering envelopes. Populated field Kod in Organisation in mapping.
</commit_message>
<xml_diff>
--- a/INT0001.Ladok2.Events/Src/Files/INT0001.Ladok2.maps.xlsx
+++ b/INT0001.Ladok2.Events/Src/Files/INT0001.Ladok2.maps.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="128">
   <si>
     <t>pnr</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t>FelVidEtableringExternt</t>
+  </si>
+  <si>
+    <t>Hämtas via MySQL anrop GetCourseDescriptions)</t>
   </si>
 </sst>
 </file>
@@ -1994,10 +1997,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD61"/>
+  <dimension ref="A1:XFD63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18950,6 +18953,22 @@
         <v>52</v>
       </c>
     </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D62" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>

</xml_diff>